<commit_message>
commit the new df_mazda
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_mazda_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_mazda_updated.xlsx
@@ -782,7 +782,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Millenia</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Millenia</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Protege</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Protege</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1034,12 +1034,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>Protege</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>No Security</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1062,17 +1062,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>B-Series (3.0L &amp; 4.0L only)</t>
+          <t>Millenia</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>PATS Type B (Stand Alone PATS Module)</t>
+          <t>No Security</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Millenia</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1118,12 +1118,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>626</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>No Security</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1146,17 +1146,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Protege</t>
+          <t>B-Series (3.0L &amp; 4.0L only)</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>No Security</t>
+          <t>PATS Type B (Stand Alone PATS Module)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>PATS Type NA (No PATS)</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Millenia</t>
+          <t>Protege</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1454,12 +1454,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Millenia</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>No Security</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1482,12 +1482,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Protege</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>No Security</t>
+          <t>PATS Type NA (No PATS)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1510,12 +1510,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>626</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1734,12 +1734,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1762,12 +1762,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>Protege</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>No Security</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1790,12 +1790,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Protege</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>No Security</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1818,12 +1818,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-B</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1874,12 +1874,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>M-B</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1958,12 +1958,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>M-B</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -1986,12 +1986,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2014,12 +2014,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>M-B</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>RX-8</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2070,12 +2070,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>B-Series (3.0L &amp; 4.0L only)</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>RX-8</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>B-Series (3.0L &amp; 4.0L only)</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2294,17 +2294,17 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>B-Series (3.0L &amp; 4.0L only)</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -2322,17 +2322,17 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>B-Series (3.0L &amp; 4.0L only)</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -2350,17 +2350,17 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>MPV</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>M-A</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -2378,12 +2378,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>MPV</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-A</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-B</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2434,12 +2434,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2462,12 +2462,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2490,17 +2490,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-B</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -2518,17 +2518,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -2546,17 +2546,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -2574,12 +2574,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>PATS Type G (Instrument Cluster)</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2602,12 +2602,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2630,17 +2630,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Tribute</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>PATS Type E (Powertrain Control Module)</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -2658,12 +2658,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2686,12 +2686,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2714,12 +2714,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -2742,17 +2742,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-B</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Tribute</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-B</t>
+          <t>PATS Type E (Powertrain Control Module)</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -2798,12 +2798,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -2826,12 +2826,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -2854,12 +2854,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Advanced Keyless: MD</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -2882,12 +2882,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -2910,17 +2910,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>PATS Type G (Instrument Cluster)</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -2938,17 +2938,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -2966,12 +2966,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -2994,12 +2994,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3022,12 +3022,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3050,17 +3050,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-B</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -3078,12 +3078,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-B</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3106,17 +3106,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -3134,12 +3134,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3162,12 +3162,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3190,12 +3190,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -3218,12 +3218,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>PATS Type G (Instrument Cluster)</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3246,12 +3246,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -3302,12 +3302,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>PATS Type G (Instrument Cluster)</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3330,12 +3330,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -3358,12 +3358,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>PATS Type G (Instrument Cluster)</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3386,12 +3386,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3414,12 +3414,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3442,12 +3442,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-E</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3470,12 +3470,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3498,12 +3498,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3526,12 +3526,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3554,12 +3554,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -3582,12 +3582,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>PATS Type G (Instrument Cluster)</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3610,12 +3610,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3666,12 +3666,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-E</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3694,12 +3694,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda3 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3722,12 +3722,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>PATS Type G (Instrument Cluster)</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3778,12 +3778,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>B-Series (2.3L, 3.0L, &amp; 4.0L)</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-E</t>
+          <t>PATS Type G (Instrument Cluster)</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -3806,12 +3806,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -3834,12 +3834,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda3 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -3862,12 +3862,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -3890,12 +3890,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -3918,12 +3918,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -3946,12 +3946,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -3974,12 +3974,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4002,12 +4002,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -4030,12 +4030,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-E</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -4058,12 +4058,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4086,12 +4086,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -4114,7 +4114,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Mazda2</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -4142,12 +4142,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-E</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -4170,12 +4170,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -4198,12 +4198,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -4226,12 +4226,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda2</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -4254,12 +4254,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -4282,12 +4282,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>RX-8 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -4310,12 +4310,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -4338,12 +4338,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -4366,12 +4366,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda3 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -4394,12 +4394,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda3 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -4422,12 +4422,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>RX-8</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -4450,12 +4450,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>RX-8 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-E</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4478,12 +4478,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Mazda2</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -4534,12 +4534,12 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>CX-7 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-E</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4562,12 +4562,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-7 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -4590,12 +4590,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -4618,12 +4618,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -4646,12 +4646,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda2</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4674,12 +4674,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -4702,12 +4702,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>Mazda3 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -4730,12 +4730,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -4758,12 +4758,12 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>CX-7</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-E</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -4786,12 +4786,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -4898,12 +4898,12 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -4926,12 +4926,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -4954,12 +4954,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -4982,12 +4982,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5010,12 +5010,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5038,12 +5038,12 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5066,12 +5066,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -5094,12 +5094,12 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5122,12 +5122,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>CX-5</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5150,12 +5150,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-5</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5178,12 +5178,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5206,12 +5206,12 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda2</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -5234,12 +5234,12 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5262,12 +5262,12 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5290,12 +5290,12 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5318,12 +5318,12 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Mazda2</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5346,12 +5346,12 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -5374,12 +5374,12 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>CX-5</t>
+          <t>MX-5 (Advanced Keyless Entry w/ Keyless Start)</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-D</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5402,12 +5402,12 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5430,12 +5430,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-9 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-F</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5458,12 +5458,12 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda2 (Keyed Ignition)</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5486,12 +5486,12 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda2 (Advanced Keyless)</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Keyless Entry w/ Keyed Ignition: M-C</t>
+          <t>M-E</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5514,12 +5514,12 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>MX-5 (Keyless Entry w/ Keyed Ignition)</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5542,12 +5542,12 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-5</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-F</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5570,12 +5570,12 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Mazda2</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Keyed Ignition: M-C</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5598,12 +5598,12 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Mazda2</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Advanced Keyless: M-E</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5626,12 +5626,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Advanced Keyless Entry w/ Keyless Start): M-D</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-3</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -5682,7 +5682,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>CX-5</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -5710,12 +5710,12 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Mazda5</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>M-C</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>CX-5</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -5766,12 +5766,12 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>Mazda5</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-C</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>CX-3</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -5850,7 +5850,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>CX-3</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -5878,7 +5878,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-3</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -5962,7 +5962,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -6018,7 +6018,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>CX-3</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>CX-3</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -6130,7 +6130,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -6158,17 +6158,17 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>CX-3</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-H</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>CX-3</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -6214,17 +6214,17 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>M-H</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -6298,17 +6298,17 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Mazda6</t>
+          <t>Mazda3</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-H</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -6326,17 +6326,17 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>CX-3</t>
+          <t>CX-30</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>M-G</t>
+          <t>M-H</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>Parameter Reset Required</t>
+          <t>Parameter Reset Not Required</t>
         </is>
       </c>
     </row>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>CX-9</t>
+          <t>MX-5 (Miata)</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -6382,17 +6382,17 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>CX-30</t>
+          <t>CX-3</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>M-H</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -6410,17 +6410,17 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Mazda3</t>
+          <t>CX-9</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>M-H</t>
+          <t>M-G</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>Parameter Reset Not Required</t>
+          <t>Parameter Reset Required</t>
         </is>
       </c>
     </row>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>MX-5 (Miata)</t>
+          <t>Mazda6</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">

</xml_diff>